<commit_message>
code ok in leetcode
</commit_message>
<xml_diff>
--- a/LeetCodeTraining/Notes/ZigzagConversion.xlsx
+++ b/LeetCodeTraining/Notes/ZigzagConversion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\__PROG__\LeetCodeTraining\LeetCodeTraining\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A7A44B-B548-435A-9BC5-266BADAD8455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAAA672-108C-4700-B7FF-238BB840DFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9E59EB3D-4284-4F2D-AE03-83E1A10D5670}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="33">
   <si>
     <t>PYAIHRNAPLSIIG</t>
   </si>
@@ -78,6 +78,63 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>AAABBBCCCDDD</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>aBc!2@#xYz</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>@</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -457,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D542FCF-878E-43A5-AF1B-2F2D152C735D}">
-  <dimension ref="C4:AX19"/>
+  <dimension ref="C4:AX25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z12" sqref="Z12"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -472,7 +529,7 @@
     <col min="51" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
@@ -483,12 +540,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="G7" s="1">
         <v>2</v>
       </c>
@@ -513,8 +573,17 @@
       <c r="N7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="R7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="H8" s="2" t="s">
         <v>5</v>
       </c>
@@ -536,8 +605,36 @@
       <c r="N8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="R8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="R10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
       <c r="G11" s="1">
         <v>3</v>
       </c>
@@ -553,8 +650,11 @@
       <c r="N11" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="R11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
       <c r="H12" s="2" t="s">
         <v>5</v>
       </c>
@@ -577,7 +677,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
       <c r="H13" s="2" t="s">
         <v>6</v>
       </c>
@@ -588,7 +688,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="R14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="R15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
       <c r="G16" s="1">
         <v>4</v>
       </c>
@@ -601,8 +717,20 @@
       <c r="N16" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="R16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H17" s="2" t="s">
         <v>5</v>
       </c>
@@ -618,8 +746,14 @@
       <c r="N17" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="R17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H18" s="2" t="s">
         <v>6</v>
       </c>
@@ -633,12 +767,56 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H19" s="2" t="s">
         <v>4</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="H25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>